<commit_message>
Added to work log
</commit_message>
<xml_diff>
--- a/Documentation/Work Log.xlsx
+++ b/Documentation/Work Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kad61\Desktop\School Things\Compsci\thing\Alexa-Text-Based-Adventure\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7606E3-EB52-4D1B-B42D-9DCDD42429E3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8714FED-5533-4EAC-92AB-BF3A627EED5C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="31">
   <si>
     <t>Date</t>
   </si>
@@ -92,6 +92,27 @@
   </si>
   <si>
     <t>Jackson &amp; Kyle</t>
+  </si>
+  <si>
+    <t>Research creating Alexa skill</t>
+  </si>
+  <si>
+    <t>2 hours</t>
+  </si>
+  <si>
+    <t>Develop the logic structure</t>
+  </si>
+  <si>
+    <t>3 hours</t>
+  </si>
+  <si>
+    <t>Connecting utterances to intents</t>
+  </si>
+  <si>
+    <t>Siddhu</t>
+  </si>
+  <si>
+    <t>1 hour</t>
   </si>
 </sst>
 </file>
@@ -99,7 +120,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -148,9 +169,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,10 +498,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -719,13 +740,72 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
+      <c r="A14" s="5">
+        <v>43621</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
+      <c r="A15" s="5">
+        <v>43621</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
+      <c r="A16" s="5">
+        <v>43621</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>43621</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:Z1000 C2:C1000 A1:B1000">

</xml_diff>

<commit_message>
Created text document with logic structure
</commit_message>
<xml_diff>
--- a/Documentation/Work Log.xlsx
+++ b/Documentation/Work Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kad61\Desktop\School Things\Compsci\thing\Alexa-Text-Based-Adventure\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8714FED-5533-4EAC-92AB-BF3A627EED5C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F876E2E-8E84-4796-B5AE-1004DD6F004E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -110,9 +110,6 @@
   </si>
   <si>
     <t>Siddhu</t>
-  </si>
-  <si>
-    <t>1 hour</t>
   </si>
 </sst>
 </file>
@@ -498,11 +495,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -764,7 +761,7 @@
         <v>26</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>8</v>
@@ -798,13 +795,30 @@
         <v>28</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>43621</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>